<commit_message>
- Signal Data Info 구성 완료 : YML, VSM 파싱 - Excel Parser 로그 추가
</commit_message>
<xml_diff>
--- a/Diagram/001_Document/Interface_Define_TC_Creator.xlsx
+++ b/Diagram/001_Document/Interface_Define_TC_Creator.xlsx
@@ -9,34 +9,35 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22905" windowHeight="14670" tabRatio="881" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22905" windowHeight="14670" tabRatio="881" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe" sheetId="27" r:id="rId1"/>
     <sheet name="추적표" sheetId="28" r:id="rId2"/>
-    <sheet name="요구사항 식별자" sheetId="23" r:id="rId3"/>
-    <sheet name="구조설계 식별자" sheetId="24" r:id="rId4"/>
-    <sheet name="상세설계 식별자" sheetId="26" r:id="rId5"/>
-    <sheet name="Detail Function" sheetId="8" r:id="rId6"/>
-    <sheet name="ControlManger" sheetId="1" r:id="rId7"/>
-    <sheet name="ScreenInfo" sheetId="3" r:id="rId8"/>
-    <sheet name="ConfigSetting" sheetId="4" r:id="rId9"/>
-    <sheet name="Util" sheetId="11" r:id="rId10"/>
-    <sheet name="Popup" sheetId="10" r:id="rId11"/>
-    <sheet name="Dialog" sheetId="21" r:id="rId12"/>
-    <sheet name="Control" sheetId="5" r:id="rId13"/>
-    <sheet name="Handler" sheetId="6" r:id="rId14"/>
-    <sheet name="Gui" sheetId="7" r:id="rId15"/>
-    <sheet name="Python" sheetId="9" r:id="rId16"/>
-    <sheet name="ControlMenu" sheetId="14" r:id="rId17"/>
-    <sheet name="HandlerMenu" sheetId="13" r:id="rId18"/>
-    <sheet name="GuiMenu" sheetId="12" r:id="rId19"/>
-    <sheet name="ControlCenter" sheetId="15" r:id="rId20"/>
-    <sheet name="HandlerCenter" sheetId="16" r:id="rId21"/>
-    <sheet name="GuiCenter" sheetId="17" r:id="rId22"/>
-    <sheet name="ControlExcel" sheetId="18" r:id="rId23"/>
-    <sheet name="HandlerExcel" sheetId="19" r:id="rId24"/>
-    <sheet name="GuiExcel" sheetId="20" r:id="rId25"/>
+    <sheet name="용어 및 약어" sheetId="29" r:id="rId3"/>
+    <sheet name="요구사항 식별자" sheetId="23" r:id="rId4"/>
+    <sheet name="구조설계 식별자" sheetId="24" r:id="rId5"/>
+    <sheet name="상세설계 식별자" sheetId="26" r:id="rId6"/>
+    <sheet name="Detail Function" sheetId="8" r:id="rId7"/>
+    <sheet name="ControlManger" sheetId="1" r:id="rId8"/>
+    <sheet name="ScreenInfo" sheetId="3" r:id="rId9"/>
+    <sheet name="ConfigSetting" sheetId="4" r:id="rId10"/>
+    <sheet name="Util" sheetId="11" r:id="rId11"/>
+    <sheet name="Popup" sheetId="10" r:id="rId12"/>
+    <sheet name="Dialog" sheetId="21" r:id="rId13"/>
+    <sheet name="Control" sheetId="5" r:id="rId14"/>
+    <sheet name="Handler" sheetId="6" r:id="rId15"/>
+    <sheet name="Gui" sheetId="7" r:id="rId16"/>
+    <sheet name="Python" sheetId="9" r:id="rId17"/>
+    <sheet name="ControlMenu" sheetId="14" r:id="rId18"/>
+    <sheet name="HandlerMenu" sheetId="13" r:id="rId19"/>
+    <sheet name="GuiMenu" sheetId="12" r:id="rId20"/>
+    <sheet name="ControlCenter" sheetId="15" r:id="rId21"/>
+    <sheet name="HandlerCenter" sheetId="16" r:id="rId22"/>
+    <sheet name="GuiCenter" sheetId="17" r:id="rId23"/>
+    <sheet name="ControlExcel" sheetId="18" r:id="rId24"/>
+    <sheet name="HandlerExcel" sheetId="19" r:id="rId25"/>
+    <sheet name="GuiExcel" sheetId="20" r:id="rId26"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -48,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1922" uniqueCount="814">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2092" uniqueCount="958">
   <si>
     <t>Description</t>
   </si>
@@ -2563,14 +2564,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>구분</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>요구사항 항목</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>SRS-REQ-0001</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -2714,14 +2707,6 @@
   </si>
   <si>
     <t>Working Path</t>
-  </si>
-  <si>
-    <t>VSM Node 표시</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>VSM Node 검색</t>
-    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>비고</t>
@@ -2921,11 +2906,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>요구사항(SRS)
-식별자</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>요구사항(SRS) 식별자</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -2964,6 +2944,462 @@
   </si>
   <si>
     <t>정보</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SRS-REQ-0001</t>
+  </si>
+  <si>
+    <t>VSM Node 표시</t>
+  </si>
+  <si>
+    <t>VSM Node 검색</t>
+  </si>
+  <si>
+    <t>SRS-REQ-0101</t>
+  </si>
+  <si>
+    <t>파싱 기능</t>
+  </si>
+  <si>
+    <t>엑셀 파일 파싱 기능</t>
+  </si>
+  <si>
+    <t>SRS-REQ-0102</t>
+  </si>
+  <si>
+    <t>VSM 파일 파싱 기능</t>
+  </si>
+  <si>
+    <t>SRS-REQ-0103</t>
+  </si>
+  <si>
+    <t>YML 파일 파싱 기능</t>
+  </si>
+  <si>
+    <t>SRS-REQ-0104</t>
+  </si>
+  <si>
+    <t>데이터 처리 기능</t>
+  </si>
+  <si>
+    <t>파싱 데이터 read/write 기능</t>
+  </si>
+  <si>
+    <t>SRS-REQ-0105</t>
+  </si>
+  <si>
+    <t>변환 데이터 read/write/erase/edit 기능</t>
+  </si>
+  <si>
+    <t>SRS-REQ-0106</t>
+  </si>
+  <si>
+    <t>Value 입력 기능</t>
+  </si>
+  <si>
+    <t>isInitialize 열 초기화 값 확인 및 설정 기능</t>
+  </si>
+  <si>
+    <t>SRS-REQ-0107</t>
+  </si>
+  <si>
+    <t>Input/Output 값 유효성 검사 기능</t>
+  </si>
+  <si>
+    <t>SRS-REQ-0108</t>
+  </si>
+  <si>
+    <t>Description 시트 정보 자동 입력 기능</t>
+  </si>
+  <si>
+    <t>SRS-REQ-0109</t>
+  </si>
+  <si>
+    <t>GenType 입력 기능</t>
+  </si>
+  <si>
+    <t>SRS-REQ-0110</t>
+  </si>
+  <si>
+    <t>자동 완성 기능</t>
+  </si>
+  <si>
+    <t>Matching table과 Value enum 자동 완성 제공 기능</t>
+  </si>
+  <si>
+    <t>SRS-REQ-0111</t>
+  </si>
+  <si>
+    <t>Manual TC 입력 정보에 대한 자동 완성 기능</t>
+  </si>
+  <si>
+    <t>SRS-REQ-0112</t>
+  </si>
+  <si>
+    <t>TCName 자동 완성 제공 기능</t>
+  </si>
+  <si>
+    <t>SRS-REQ-0113</t>
+  </si>
+  <si>
+    <t>TCName Result 값 자동 완성 제공 기능</t>
+  </si>
+  <si>
+    <t>SRS-REQ-0114</t>
+  </si>
+  <si>
+    <t>사양서 기반 키워드 지원 기능</t>
+  </si>
+  <si>
+    <t>Value Changed 키워드 기능</t>
+  </si>
+  <si>
+    <t>SRS-REQ-0115</t>
+  </si>
+  <si>
+    <t>[Sheet] 키워드 기능</t>
+  </si>
+  <si>
+    <t>SRS-REQ-0116</t>
+  </si>
+  <si>
+    <t>쉼표(,) 키워드 기능</t>
+  </si>
+  <si>
+    <t>SRS-REQ-0117</t>
+  </si>
+  <si>
+    <t>범위(~) 키워드 기능</t>
+  </si>
+  <si>
+    <t>SRS-REQ-0118</t>
+  </si>
+  <si>
+    <t>초과(&gt;) 키워드 기능</t>
+  </si>
+  <si>
+    <t>SRS-REQ-0119</t>
+  </si>
+  <si>
+    <t>미만(&lt;) 키워드 기능</t>
+  </si>
+  <si>
+    <t>SRS-REQ-0120</t>
+  </si>
+  <si>
+    <t>이상(&gt;=) 키워드 기능</t>
+  </si>
+  <si>
+    <t>SRS-REQ-0121</t>
+  </si>
+  <si>
+    <t>이하(&lt;=) 키워드 기능</t>
+  </si>
+  <si>
+    <t>SRS-REQ-0122</t>
+  </si>
+  <si>
+    <t>SRS-REQ-0123</t>
+  </si>
+  <si>
+    <t>NOT (!) 키워드 기능</t>
+  </si>
+  <si>
+    <t>SRS-REQ-0124</t>
+  </si>
+  <si>
+    <t>Don’t care(D`) 키워드 기능</t>
+  </si>
+  <si>
+    <t>SRS-REQ-0125</t>
+  </si>
+  <si>
+    <t>timeout, MESSAGE_TIMEOUT 키워드 기능</t>
+  </si>
+  <si>
+    <t>SRS-REQ-0126</t>
+  </si>
+  <si>
+    <t>crc, CRC_ERROR 키워드 기능</t>
+  </si>
+  <si>
+    <t>SRS-REQ-0127</t>
+  </si>
+  <si>
+    <t>[Cal] 키워드 기능</t>
+  </si>
+  <si>
+    <t>SRS-REQ-0128</t>
+  </si>
+  <si>
+    <t>사용자 지정 기반 키워드 지원 기능</t>
+  </si>
+  <si>
+    <t>[NOT_TRIGGER] 키워드 기능</t>
+  </si>
+  <si>
+    <t>SRS-REQ-0129</t>
+  </si>
+  <si>
+    <t>[PRESET] 키워드 기능</t>
+  </si>
+  <si>
+    <t>SRS-REQ-0130</t>
+  </si>
+  <si>
+    <t>[DEPENDENT_ON] 키워드 기능</t>
+  </si>
+  <si>
+    <t>SRS-REQ-0131</t>
+  </si>
+  <si>
+    <t>Case 생성 기능</t>
+  </si>
+  <si>
+    <t>Result 열 기준 동일 값 처리 기능</t>
+  </si>
+  <si>
+    <t>SRS-REQ-0132</t>
+  </si>
+  <si>
+    <t>Default 생성 기능</t>
+  </si>
+  <si>
+    <t>SRS-REQ-0133</t>
+  </si>
+  <si>
+    <t>Negative(+Positive) 생성 기능</t>
+  </si>
+  <si>
+    <t>SRS-REQ-0134</t>
+  </si>
+  <si>
+    <t>엑셀 작성 순서 정렬 기능</t>
+  </si>
+  <si>
+    <t>SRS-REQ-0135</t>
+  </si>
+  <si>
+    <t>TC 파일 생성 기능</t>
+  </si>
+  <si>
+    <t>초기화(init)값 TC 생성 기능</t>
+  </si>
+  <si>
+    <t>SRS-REQ-0136</t>
+  </si>
+  <si>
+    <t>Result 열 기준 동일 값 TC 생성 기능</t>
+  </si>
+  <si>
+    <t>SRS-REQ-0137</t>
+  </si>
+  <si>
+    <t>config 값 TC 생성 기능</t>
+  </si>
+  <si>
+    <t>SRS-REQ-0138</t>
+  </si>
+  <si>
+    <t>TC파일내 고유 TC 명(name) 생성 기능</t>
+  </si>
+  <si>
+    <t>SRS-REQ-0139</t>
+  </si>
+  <si>
+    <t>AEM_init값 TC 생성 기능</t>
+  </si>
+  <si>
+    <t>SRS-REQ-0140</t>
+  </si>
+  <si>
+    <t>timeout, dump값 TC 생성 기능</t>
+  </si>
+  <si>
+    <t>SRS-REQ-0141</t>
+  </si>
+  <si>
+    <t>유효한 enum 값 기반 TC 생성 기능</t>
+  </si>
+  <si>
+    <t>SRS-REQ-0142</t>
+  </si>
+  <si>
+    <t>Private 시트 TC 생성 기능</t>
+  </si>
+  <si>
+    <t>SRS-REQ-0143</t>
+  </si>
+  <si>
+    <t>사용자 선택 항목(TCName) 기준 TC 생성 기능</t>
+  </si>
+  <si>
+    <t>SRS-REQ-0144</t>
+  </si>
+  <si>
+    <t>Manual TC 시트 정보 TC 생성 기능</t>
+  </si>
+  <si>
+    <t>SRS-REQ-0145</t>
+  </si>
+  <si>
+    <t>DEPENDENT_ON 데이터 TC 생성 기능</t>
+  </si>
+  <si>
+    <t>SRS-REQ-0146</t>
+  </si>
+  <si>
+    <t>시그널 값 주석 기재 기능</t>
+  </si>
+  <si>
+    <t>SRS-REQ-0147</t>
+  </si>
+  <si>
+    <t>팝업 표시 기능</t>
+  </si>
+  <si>
+    <t>입력 데이터 오류(자료형) 팝업 기능</t>
+  </si>
+  <si>
+    <t>SRS-REQ-0148</t>
+  </si>
+  <si>
+    <t>TC 케이스 생성 오류 팝업 기능</t>
+  </si>
+  <si>
+    <t>SRS-REQ-0149</t>
+  </si>
+  <si>
+    <t>로그 출력 기능</t>
+  </si>
+  <si>
+    <t>유효하지 않은 enum 값 미생성 정보 로그 출력 기능</t>
+  </si>
+  <si>
+    <t>SRS-REQ-0150</t>
+  </si>
+  <si>
+    <t>SRS-REQ-0151</t>
+  </si>
+  <si>
+    <t>Validator 동작 기능</t>
+  </si>
+  <si>
+    <t>SRS-REQ-0152</t>
+  </si>
+  <si>
+    <t>화면 표시 기능</t>
+  </si>
+  <si>
+    <t>사용자 선택 항목(TCName열) 체크 기능</t>
+  </si>
+  <si>
+    <t>SRS-REQ-0153</t>
+  </si>
+  <si>
+    <t>메뉴 항목 (Multi Docker Run) 선택 기능</t>
+  </si>
+  <si>
+    <t>SRS-REQ-0154</t>
+  </si>
+  <si>
+    <t>도커 실행 상태 표시 기능</t>
+  </si>
+  <si>
+    <t>SRS-REQ-0155</t>
+  </si>
+  <si>
+    <t>도커 동작 기능</t>
+  </si>
+  <si>
+    <t>도커 실행 상태 확인 기능</t>
+  </si>
+  <si>
+    <t>SRS-REQ-0156</t>
+  </si>
+  <si>
+    <t>멀티 도커 기반 RunTC 동작 기능</t>
+  </si>
+  <si>
+    <t>SRS-REQ-0157</t>
+  </si>
+  <si>
+    <t>멀티 도커 동작 옵션 제공 기능</t>
+  </si>
+  <si>
+    <t>SRS-REQ-0158</t>
+  </si>
+  <si>
+    <t>기타 기능</t>
+  </si>
+  <si>
+    <t>엑셀 파일 열 명칭 변경</t>
+  </si>
+  <si>
+    <t>SRS-REQ-0159</t>
+  </si>
+  <si>
+    <t>스크립트 명령어 옵션 변경</t>
+  </si>
+  <si>
+    <t>SRS-REQ-0160</t>
+  </si>
+  <si>
+    <t>용어 변경</t>
+  </si>
+  <si>
+    <t>SRS-REQ-0101 ~</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>TBD</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>요구사항(SRS)식별자</t>
+  </si>
+  <si>
+    <t>구분</t>
+  </si>
+  <si>
+    <t>요구사항 항목</t>
+  </si>
+  <si>
+    <t>FLOW (=&gt;) 키워드 기능</t>
+  </si>
+  <si>
+    <t>TCName열 기준 케이스별 TC 생성 정보 로그 출력 기능</t>
+  </si>
+  <si>
+    <t>TC 파일 작성 순서(signal/value) 기반 동작 기능</t>
+  </si>
+  <si>
+    <t>SRS-REQ-0161</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SRS-REQ-0162</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Others 키워드 기능 (Others 케이스 생성 기능)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CLI 동작 기능 검토 (TBD)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>설명</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>용어</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>약어</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -2971,7 +3407,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3020,6 +3456,21 @@
       <family val="3"/>
       <charset val="129"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -3041,7 +3492,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -3101,50 +3552,13 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -3184,9 +3598,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -3199,13 +3610,49 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3226,25 +3673,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -3535,78 +3964,78 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.625" style="33" customWidth="1"/>
-    <col min="2" max="2" width="23.25" style="33" customWidth="1"/>
-    <col min="3" max="3" width="67.25" style="33" customWidth="1"/>
-    <col min="4" max="16384" width="9" style="33"/>
+    <col min="1" max="1" width="2.625" style="22" customWidth="1"/>
+    <col min="2" max="2" width="23.25" style="22" customWidth="1"/>
+    <col min="3" max="3" width="67.25" style="22" customWidth="1"/>
+    <col min="4" max="16384" width="9" style="22"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B2" s="27" t="s">
-        <v>812</v>
-      </c>
-      <c r="C2" s="27" t="s">
-        <v>813</v>
+      <c r="B2" s="17" t="s">
+        <v>807</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>808</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B3" s="31" t="s">
+      <c r="B3" s="29" t="s">
+        <v>772</v>
+      </c>
+      <c r="C3" s="21" t="s">
+        <v>773</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B4" s="29"/>
+      <c r="C4" s="21" t="s">
+        <v>774</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B5" s="29"/>
+      <c r="C5" s="21" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B6" s="29" t="s">
+        <v>775</v>
+      </c>
+      <c r="C6" s="21" t="s">
         <v>776</v>
       </c>
-      <c r="C3" s="32" t="s">
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B7" s="29"/>
+      <c r="C7" s="21" t="s">
         <v>777</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B4" s="31"/>
-      <c r="C4" s="32" t="s">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B8" s="29"/>
+      <c r="C8" s="21" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B9" s="29" t="s">
         <v>778</v>
       </c>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B5" s="31"/>
-      <c r="C5" s="32" t="s">
-        <v>694</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B6" s="31" t="s">
+      <c r="C9" s="21" t="s">
         <v>779</v>
       </c>
-      <c r="C6" s="32" t="s">
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B10" s="29"/>
+      <c r="C10" s="21" t="s">
         <v>780</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B7" s="31"/>
-      <c r="C7" s="32" t="s">
-        <v>781</v>
-      </c>
-    </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B8" s="31"/>
-      <c r="C8" s="32" t="s">
-        <v>755</v>
-      </c>
-    </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B9" s="31" t="s">
-        <v>782</v>
-      </c>
-      <c r="C9" s="32" t="s">
-        <v>783</v>
-      </c>
-    </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B10" s="31"/>
-      <c r="C10" s="32" t="s">
-        <v>784</v>
-      </c>
-    </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B11" s="31"/>
-      <c r="C11" s="32" t="s">
-        <v>746</v>
+      <c r="B11" s="29"/>
+      <c r="C11" s="21" t="s">
+        <v>742</v>
       </c>
     </row>
   </sheetData>
@@ -3622,6 +4051,212 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D13"/>
+  <sheetViews>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39.625" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="9" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="27" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="27" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="27" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="27" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D13"/>
   <sheetViews>
@@ -3731,7 +4366,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D12"/>
   <sheetViews>
@@ -3923,7 +4558,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D67"/>
   <sheetViews>
@@ -4444,10 +5079,10 @@
       </c>
     </row>
     <row r="37" spans="1:4" ht="100.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="24"/>
-      <c r="B37" s="25"/>
-      <c r="C37" s="25"/>
-      <c r="D37" s="26"/>
+      <c r="A37" s="35"/>
+      <c r="B37" s="36"/>
+      <c r="C37" s="36"/>
+      <c r="D37" s="37"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
@@ -4879,7 +5514,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D26"/>
   <sheetViews>
@@ -5267,7 +5902,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D14"/>
   <sheetViews>
@@ -5487,7 +6122,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D10"/>
   <sheetViews>
@@ -5651,7 +6286,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D8"/>
   <sheetViews>
@@ -5773,7 +6408,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D41"/>
   <sheetViews>
@@ -6371,7 +7006,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D14"/>
   <sheetViews>
@@ -6591,7 +7226,329 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D25"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="13.25" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="16384" width="13.25" style="19"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="27" x14ac:dyDescent="0.3">
+      <c r="A1" s="17" t="s">
+        <v>797</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>798</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>799</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="27" x14ac:dyDescent="0.3">
+      <c r="A2" s="18" t="s">
+        <v>692</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>800</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>944</v>
+      </c>
+      <c r="D2" s="20"/>
+    </row>
+    <row r="3" spans="1:4" ht="27" x14ac:dyDescent="0.3">
+      <c r="A3" s="18" t="s">
+        <v>693</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>800</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>944</v>
+      </c>
+      <c r="D3" s="20"/>
+    </row>
+    <row r="4" spans="1:4" ht="94.5" x14ac:dyDescent="0.3">
+      <c r="A4" s="18" t="s">
+        <v>694</v>
+      </c>
+      <c r="B4" s="20" t="s">
+        <v>801</v>
+      </c>
+      <c r="C4" s="20" t="s">
+        <v>944</v>
+      </c>
+      <c r="D4" s="20"/>
+    </row>
+    <row r="5" spans="1:4" ht="40.5" x14ac:dyDescent="0.3">
+      <c r="A5" s="18" t="s">
+        <v>695</v>
+      </c>
+      <c r="B5" s="20" t="s">
+        <v>802</v>
+      </c>
+      <c r="C5" s="20" t="s">
+        <v>944</v>
+      </c>
+      <c r="D5" s="20"/>
+    </row>
+    <row r="6" spans="1:4" ht="40.5" x14ac:dyDescent="0.3">
+      <c r="A6" s="18" t="s">
+        <v>696</v>
+      </c>
+      <c r="B6" s="20" t="s">
+        <v>802</v>
+      </c>
+      <c r="C6" s="20" t="s">
+        <v>944</v>
+      </c>
+      <c r="D6" s="20"/>
+    </row>
+    <row r="7" spans="1:4" ht="40.5" x14ac:dyDescent="0.3">
+      <c r="A7" s="18" t="s">
+        <v>697</v>
+      </c>
+      <c r="B7" s="20" t="s">
+        <v>802</v>
+      </c>
+      <c r="C7" s="20" t="s">
+        <v>944</v>
+      </c>
+      <c r="D7" s="20"/>
+    </row>
+    <row r="8" spans="1:4" ht="40.5" x14ac:dyDescent="0.3">
+      <c r="A8" s="18" t="s">
+        <v>698</v>
+      </c>
+      <c r="B8" s="20" t="s">
+        <v>802</v>
+      </c>
+      <c r="C8" s="20" t="s">
+        <v>944</v>
+      </c>
+      <c r="D8" s="20"/>
+    </row>
+    <row r="9" spans="1:4" ht="40.5" x14ac:dyDescent="0.3">
+      <c r="A9" s="18" t="s">
+        <v>699</v>
+      </c>
+      <c r="B9" s="20" t="s">
+        <v>802</v>
+      </c>
+      <c r="C9" s="20" t="s">
+        <v>944</v>
+      </c>
+      <c r="D9" s="20"/>
+    </row>
+    <row r="10" spans="1:4" ht="40.5" x14ac:dyDescent="0.3">
+      <c r="A10" s="18" t="s">
+        <v>700</v>
+      </c>
+      <c r="B10" s="20" t="s">
+        <v>802</v>
+      </c>
+      <c r="C10" s="20" t="s">
+        <v>944</v>
+      </c>
+      <c r="D10" s="20"/>
+    </row>
+    <row r="11" spans="1:4" ht="40.5" x14ac:dyDescent="0.3">
+      <c r="A11" s="18" t="s">
+        <v>701</v>
+      </c>
+      <c r="B11" s="20" t="s">
+        <v>802</v>
+      </c>
+      <c r="C11" s="20" t="s">
+        <v>944</v>
+      </c>
+      <c r="D11" s="20"/>
+    </row>
+    <row r="12" spans="1:4" ht="54" x14ac:dyDescent="0.3">
+      <c r="A12" s="18" t="s">
+        <v>702</v>
+      </c>
+      <c r="B12" s="20" t="s">
+        <v>803</v>
+      </c>
+      <c r="C12" s="20" t="s">
+        <v>944</v>
+      </c>
+      <c r="D12" s="20"/>
+    </row>
+    <row r="13" spans="1:4" ht="81" x14ac:dyDescent="0.3">
+      <c r="A13" s="18" t="s">
+        <v>703</v>
+      </c>
+      <c r="B13" s="20" t="s">
+        <v>804</v>
+      </c>
+      <c r="C13" s="20" t="s">
+        <v>944</v>
+      </c>
+      <c r="D13" s="20"/>
+    </row>
+    <row r="14" spans="1:4" ht="81" x14ac:dyDescent="0.3">
+      <c r="A14" s="18" t="s">
+        <v>704</v>
+      </c>
+      <c r="B14" s="20" t="s">
+        <v>804</v>
+      </c>
+      <c r="C14" s="20" t="s">
+        <v>944</v>
+      </c>
+      <c r="D14" s="20"/>
+    </row>
+    <row r="15" spans="1:4" ht="40.5" x14ac:dyDescent="0.3">
+      <c r="A15" s="18" t="s">
+        <v>705</v>
+      </c>
+      <c r="B15" s="20" t="s">
+        <v>802</v>
+      </c>
+      <c r="C15" s="20" t="s">
+        <v>944</v>
+      </c>
+      <c r="D15" s="20"/>
+    </row>
+    <row r="16" spans="1:4" ht="67.5" x14ac:dyDescent="0.3">
+      <c r="A16" s="18" t="s">
+        <v>706</v>
+      </c>
+      <c r="B16" s="20" t="s">
+        <v>805</v>
+      </c>
+      <c r="C16" s="20" t="s">
+        <v>944</v>
+      </c>
+      <c r="D16" s="20"/>
+    </row>
+    <row r="17" spans="1:4" ht="67.5" x14ac:dyDescent="0.3">
+      <c r="A17" s="18" t="s">
+        <v>707</v>
+      </c>
+      <c r="B17" s="20" t="s">
+        <v>805</v>
+      </c>
+      <c r="C17" s="20" t="s">
+        <v>944</v>
+      </c>
+      <c r="D17" s="20"/>
+    </row>
+    <row r="18" spans="1:4" ht="67.5" x14ac:dyDescent="0.3">
+      <c r="A18" s="18" t="s">
+        <v>708</v>
+      </c>
+      <c r="B18" s="20" t="s">
+        <v>805</v>
+      </c>
+      <c r="C18" s="20" t="s">
+        <v>944</v>
+      </c>
+      <c r="D18" s="20"/>
+    </row>
+    <row r="19" spans="1:4" ht="67.5" x14ac:dyDescent="0.3">
+      <c r="A19" s="18" t="s">
+        <v>709</v>
+      </c>
+      <c r="B19" s="20" t="s">
+        <v>805</v>
+      </c>
+      <c r="C19" s="20" t="s">
+        <v>944</v>
+      </c>
+      <c r="D19" s="20"/>
+    </row>
+    <row r="20" spans="1:4" ht="67.5" x14ac:dyDescent="0.3">
+      <c r="A20" s="18" t="s">
+        <v>710</v>
+      </c>
+      <c r="B20" s="20" t="s">
+        <v>805</v>
+      </c>
+      <c r="C20" s="20" t="s">
+        <v>944</v>
+      </c>
+      <c r="D20" s="20"/>
+    </row>
+    <row r="21" spans="1:4" ht="54" x14ac:dyDescent="0.3">
+      <c r="A21" s="18" t="s">
+        <v>711</v>
+      </c>
+      <c r="B21" s="20" t="s">
+        <v>803</v>
+      </c>
+      <c r="C21" s="20" t="s">
+        <v>944</v>
+      </c>
+      <c r="D21" s="20"/>
+    </row>
+    <row r="22" spans="1:4" ht="54" x14ac:dyDescent="0.3">
+      <c r="A22" s="18" t="s">
+        <v>712</v>
+      </c>
+      <c r="B22" s="20" t="s">
+        <v>803</v>
+      </c>
+      <c r="C22" s="20" t="s">
+        <v>944</v>
+      </c>
+      <c r="D22" s="20"/>
+    </row>
+    <row r="23" spans="1:4" ht="67.5" x14ac:dyDescent="0.3">
+      <c r="A23" s="18" t="s">
+        <v>713</v>
+      </c>
+      <c r="B23" s="20" t="s">
+        <v>806</v>
+      </c>
+      <c r="C23" s="20" t="s">
+        <v>944</v>
+      </c>
+      <c r="D23" s="20"/>
+    </row>
+    <row r="24" spans="1:4" ht="67.5" x14ac:dyDescent="0.3">
+      <c r="A24" s="18" t="s">
+        <v>714</v>
+      </c>
+      <c r="B24" s="20" t="s">
+        <v>806</v>
+      </c>
+      <c r="C24" s="20" t="s">
+        <v>944</v>
+      </c>
+      <c r="D24" s="20"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="18" t="s">
+        <v>943</v>
+      </c>
+      <c r="B25" s="20" t="s">
+        <v>944</v>
+      </c>
+      <c r="C25" s="20" t="s">
+        <v>944</v>
+      </c>
+      <c r="D25" s="20"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D36"/>
   <sheetViews>
@@ -7119,271 +8076,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D24"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="13.25" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="16384" width="13.25" style="29"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" ht="27" x14ac:dyDescent="0.3">
-      <c r="A1" s="27" t="s">
-        <v>802</v>
-      </c>
-      <c r="B1" s="27" t="s">
-        <v>803</v>
-      </c>
-      <c r="C1" s="27" t="s">
-        <v>804</v>
-      </c>
-      <c r="D1" s="27" t="s">
-        <v>785</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="27" x14ac:dyDescent="0.3">
-      <c r="A2" s="28" t="s">
-        <v>694</v>
-      </c>
-      <c r="B2" s="30" t="s">
-        <v>805</v>
-      </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-    </row>
-    <row r="3" spans="1:4" ht="27" x14ac:dyDescent="0.3">
-      <c r="A3" s="28" t="s">
-        <v>695</v>
-      </c>
-      <c r="B3" s="30" t="s">
-        <v>805</v>
-      </c>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-    </row>
-    <row r="4" spans="1:4" ht="94.5" x14ac:dyDescent="0.3">
-      <c r="A4" s="28" t="s">
-        <v>696</v>
-      </c>
-      <c r="B4" s="30" t="s">
-        <v>806</v>
-      </c>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30"/>
-    </row>
-    <row r="5" spans="1:4" ht="40.5" x14ac:dyDescent="0.3">
-      <c r="A5" s="28" t="s">
-        <v>697</v>
-      </c>
-      <c r="B5" s="30" t="s">
-        <v>807</v>
-      </c>
-      <c r="C5" s="30"/>
-      <c r="D5" s="30"/>
-    </row>
-    <row r="6" spans="1:4" ht="40.5" x14ac:dyDescent="0.3">
-      <c r="A6" s="28" t="s">
-        <v>698</v>
-      </c>
-      <c r="B6" s="30" t="s">
-        <v>807</v>
-      </c>
-      <c r="C6" s="30"/>
-      <c r="D6" s="30"/>
-    </row>
-    <row r="7" spans="1:4" ht="40.5" x14ac:dyDescent="0.3">
-      <c r="A7" s="28" t="s">
-        <v>699</v>
-      </c>
-      <c r="B7" s="30" t="s">
-        <v>807</v>
-      </c>
-      <c r="C7" s="30"/>
-      <c r="D7" s="30"/>
-    </row>
-    <row r="8" spans="1:4" ht="40.5" x14ac:dyDescent="0.3">
-      <c r="A8" s="28" t="s">
-        <v>700</v>
-      </c>
-      <c r="B8" s="30" t="s">
-        <v>807</v>
-      </c>
-      <c r="C8" s="30"/>
-      <c r="D8" s="30"/>
-    </row>
-    <row r="9" spans="1:4" ht="40.5" x14ac:dyDescent="0.3">
-      <c r="A9" s="28" t="s">
-        <v>701</v>
-      </c>
-      <c r="B9" s="30" t="s">
-        <v>807</v>
-      </c>
-      <c r="C9" s="30"/>
-      <c r="D9" s="30"/>
-    </row>
-    <row r="10" spans="1:4" ht="40.5" x14ac:dyDescent="0.3">
-      <c r="A10" s="28" t="s">
-        <v>702</v>
-      </c>
-      <c r="B10" s="30" t="s">
-        <v>807</v>
-      </c>
-      <c r="C10" s="30"/>
-      <c r="D10" s="30"/>
-    </row>
-    <row r="11" spans="1:4" ht="40.5" x14ac:dyDescent="0.3">
-      <c r="A11" s="28" t="s">
-        <v>703</v>
-      </c>
-      <c r="B11" s="30" t="s">
-        <v>807</v>
-      </c>
-      <c r="C11" s="30"/>
-      <c r="D11" s="30"/>
-    </row>
-    <row r="12" spans="1:4" ht="54" x14ac:dyDescent="0.3">
-      <c r="A12" s="28" t="s">
-        <v>704</v>
-      </c>
-      <c r="B12" s="30" t="s">
-        <v>808</v>
-      </c>
-      <c r="C12" s="30"/>
-      <c r="D12" s="30"/>
-    </row>
-    <row r="13" spans="1:4" ht="81" x14ac:dyDescent="0.3">
-      <c r="A13" s="28" t="s">
-        <v>705</v>
-      </c>
-      <c r="B13" s="30" t="s">
-        <v>809</v>
-      </c>
-      <c r="C13" s="30"/>
-      <c r="D13" s="30"/>
-    </row>
-    <row r="14" spans="1:4" ht="81" x14ac:dyDescent="0.3">
-      <c r="A14" s="28" t="s">
-        <v>706</v>
-      </c>
-      <c r="B14" s="30" t="s">
-        <v>809</v>
-      </c>
-      <c r="C14" s="30"/>
-      <c r="D14" s="30"/>
-    </row>
-    <row r="15" spans="1:4" ht="40.5" x14ac:dyDescent="0.3">
-      <c r="A15" s="28" t="s">
-        <v>707</v>
-      </c>
-      <c r="B15" s="30" t="s">
-        <v>807</v>
-      </c>
-      <c r="C15" s="30"/>
-      <c r="D15" s="30"/>
-    </row>
-    <row r="16" spans="1:4" ht="67.5" x14ac:dyDescent="0.3">
-      <c r="A16" s="28" t="s">
-        <v>708</v>
-      </c>
-      <c r="B16" s="30" t="s">
-        <v>810</v>
-      </c>
-      <c r="C16" s="30"/>
-      <c r="D16" s="30"/>
-    </row>
-    <row r="17" spans="1:4" ht="67.5" x14ac:dyDescent="0.3">
-      <c r="A17" s="28" t="s">
-        <v>709</v>
-      </c>
-      <c r="B17" s="30" t="s">
-        <v>810</v>
-      </c>
-      <c r="C17" s="30"/>
-      <c r="D17" s="30"/>
-    </row>
-    <row r="18" spans="1:4" ht="67.5" x14ac:dyDescent="0.3">
-      <c r="A18" s="28" t="s">
-        <v>710</v>
-      </c>
-      <c r="B18" s="30" t="s">
-        <v>810</v>
-      </c>
-      <c r="C18" s="30"/>
-      <c r="D18" s="30"/>
-    </row>
-    <row r="19" spans="1:4" ht="67.5" x14ac:dyDescent="0.3">
-      <c r="A19" s="28" t="s">
-        <v>711</v>
-      </c>
-      <c r="B19" s="30" t="s">
-        <v>810</v>
-      </c>
-      <c r="C19" s="30"/>
-      <c r="D19" s="30"/>
-    </row>
-    <row r="20" spans="1:4" ht="67.5" x14ac:dyDescent="0.3">
-      <c r="A20" s="28" t="s">
-        <v>712</v>
-      </c>
-      <c r="B20" s="30" t="s">
-        <v>810</v>
-      </c>
-      <c r="C20" s="30"/>
-      <c r="D20" s="30"/>
-    </row>
-    <row r="21" spans="1:4" ht="54" x14ac:dyDescent="0.3">
-      <c r="A21" s="28" t="s">
-        <v>713</v>
-      </c>
-      <c r="B21" s="30" t="s">
-        <v>808</v>
-      </c>
-      <c r="C21" s="30"/>
-      <c r="D21" s="30"/>
-    </row>
-    <row r="22" spans="1:4" ht="54" x14ac:dyDescent="0.3">
-      <c r="A22" s="28" t="s">
-        <v>714</v>
-      </c>
-      <c r="B22" s="30" t="s">
-        <v>808</v>
-      </c>
-      <c r="C22" s="30"/>
-      <c r="D22" s="30"/>
-    </row>
-    <row r="23" spans="1:4" ht="67.5" x14ac:dyDescent="0.3">
-      <c r="A23" s="28" t="s">
-        <v>715</v>
-      </c>
-      <c r="B23" s="30" t="s">
-        <v>811</v>
-      </c>
-      <c r="C23" s="30"/>
-      <c r="D23" s="30"/>
-    </row>
-    <row r="24" spans="1:4" ht="67.5" x14ac:dyDescent="0.3">
-      <c r="A24" s="28" t="s">
-        <v>716</v>
-      </c>
-      <c r="B24" s="30" t="s">
-        <v>811</v>
-      </c>
-      <c r="C24" s="30"/>
-      <c r="D24" s="30"/>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D35"/>
   <sheetViews>
@@ -7897,7 +8590,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D14"/>
   <sheetViews>
@@ -8117,7 +8810,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D21"/>
   <sheetViews>
@@ -8435,7 +9128,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D42"/>
   <sheetViews>
@@ -9047,7 +9740,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D14"/>
   <sheetViews>
@@ -9267,7 +9960,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D43"/>
   <sheetViews>
@@ -9895,282 +10588,1118 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C3"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.875" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.25" style="2" customWidth="1"/>
+    <col min="2" max="2" width="48.25" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.25" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="9" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="17" t="s">
+        <v>956</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>955</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="27"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="27"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="27"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="25"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="27"/>
+      <c r="B5" s="25"/>
+      <c r="C5" s="25"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="27"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="25"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="27"/>
+      <c r="B7" s="25"/>
+      <c r="C7" s="25"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="27"/>
+      <c r="B8" s="25"/>
+      <c r="C8" s="25"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="27"/>
+      <c r="B9" s="25"/>
+      <c r="C9" s="25"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="27"/>
+      <c r="B10" s="25"/>
+      <c r="C10" s="25"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="27"/>
+      <c r="B11" s="25"/>
+      <c r="C11" s="25"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="27"/>
+      <c r="B12" s="25"/>
+      <c r="C12" s="25"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="27"/>
+      <c r="B13" s="25"/>
+      <c r="C13" s="25"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="27"/>
+      <c r="B14" s="25"/>
+      <c r="C14" s="25"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="17" t="s">
+        <v>957</v>
+      </c>
+      <c r="B17" s="17" t="s">
+        <v>955</v>
+      </c>
+      <c r="C17" s="17" t="s">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="27"/>
+      <c r="B18" s="25"/>
+      <c r="C18" s="25"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="27"/>
+      <c r="B19" s="25"/>
+      <c r="C19" s="25"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="27"/>
+      <c r="B20" s="25"/>
+      <c r="C20" s="25"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="27"/>
+      <c r="B21" s="25"/>
+      <c r="C21" s="25"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="27"/>
+      <c r="B22" s="25"/>
+      <c r="C22" s="25"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="27"/>
+      <c r="B23" s="25"/>
+      <c r="C23" s="25"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="27"/>
+      <c r="B24" s="25"/>
+      <c r="C24" s="25"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="27"/>
+      <c r="B25" s="25"/>
+      <c r="C25" s="25"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="27"/>
+      <c r="B26" s="25"/>
+      <c r="C26" s="25"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="27"/>
+      <c r="B27" s="25"/>
+      <c r="C27" s="25"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="27"/>
+      <c r="B28" s="25"/>
+      <c r="C28" s="25"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="27"/>
+      <c r="B29" s="25"/>
+      <c r="C29" s="25"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="27"/>
+      <c r="B30" s="25"/>
+      <c r="C30" s="25"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D86"/>
+  <sheetViews>
+    <sheetView topLeftCell="A55" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C87" sqref="C87"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.25" style="2" customWidth="1"/>
     <col min="2" max="2" width="19.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.75" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="48.25" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27.25" style="2" customWidth="1"/>
     <col min="5" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="27" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
-        <v>801</v>
-      </c>
-      <c r="B1" s="13" t="s">
-        <v>692</v>
-      </c>
-      <c r="C1" s="13" t="s">
+      <c r="A1" s="17" t="s">
+        <v>945</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>946</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>947</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="23" t="s">
+        <v>809</v>
+      </c>
+      <c r="B2" s="31" t="s">
+        <v>715</v>
+      </c>
+      <c r="C2" s="24" t="s">
+        <v>716</v>
+      </c>
+      <c r="D2" s="25"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="23" t="s">
         <v>693</v>
       </c>
-      <c r="D1" s="13" t="s">
-        <v>744</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="16" t="s">
+      <c r="B3" s="31"/>
+      <c r="C3" s="25" t="s">
+        <v>717</v>
+      </c>
+      <c r="D3" s="25"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="23" t="s">
         <v>694</v>
       </c>
-      <c r="B2" s="18" t="s">
-        <v>717</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="B4" s="31" t="s">
         <v>718</v>
       </c>
-      <c r="D2" s="3"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="16" t="s">
+      <c r="C4" s="25" t="s">
+        <v>719</v>
+      </c>
+      <c r="D4" s="25"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="23" t="s">
         <v>695</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="3" t="s">
-        <v>719</v>
-      </c>
-      <c r="D3" s="3"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="16" t="s">
+      <c r="B5" s="31"/>
+      <c r="C5" s="25" t="s">
+        <v>720</v>
+      </c>
+      <c r="D5" s="25"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="23" t="s">
         <v>696</v>
       </c>
-      <c r="B4" s="18" t="s">
-        <v>720</v>
-      </c>
-      <c r="C4" s="3" t="s">
+      <c r="B6" s="31"/>
+      <c r="C6" s="25" t="s">
         <v>721</v>
       </c>
-      <c r="D4" s="3"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="16" t="s">
+      <c r="D6" s="25"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="23" t="s">
         <v>697</v>
       </c>
-      <c r="B5" s="20"/>
-      <c r="C5" s="3" t="s">
+      <c r="B7" s="31"/>
+      <c r="C7" s="25" t="s">
         <v>722</v>
       </c>
-      <c r="D5" s="3"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="16" t="s">
+      <c r="D7" s="25"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="23" t="s">
         <v>698</v>
       </c>
-      <c r="B6" s="20"/>
-      <c r="C6" s="3" t="s">
+      <c r="B8" s="31"/>
+      <c r="C8" s="25" t="s">
         <v>723</v>
       </c>
-      <c r="D6" s="3"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="16" t="s">
+      <c r="D8" s="25"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="23" t="s">
         <v>699</v>
       </c>
-      <c r="B7" s="20"/>
-      <c r="C7" s="3" t="s">
+      <c r="B9" s="31"/>
+      <c r="C9" s="25" t="s">
         <v>724</v>
       </c>
-      <c r="D7" s="3"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="16" t="s">
+      <c r="D9" s="25"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="23" t="s">
         <v>700</v>
       </c>
-      <c r="B8" s="20"/>
-      <c r="C8" s="3" t="s">
+      <c r="B10" s="31"/>
+      <c r="C10" s="25" t="s">
         <v>725</v>
       </c>
-      <c r="D8" s="3"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="16" t="s">
+      <c r="D10" s="25"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="23" t="s">
         <v>701</v>
       </c>
-      <c r="B9" s="20"/>
-      <c r="C9" s="3" t="s">
+      <c r="B11" s="31"/>
+      <c r="C11" s="25" t="s">
         <v>726</v>
       </c>
-      <c r="D9" s="3"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="16" t="s">
+      <c r="D11" s="25"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="23" t="s">
         <v>702</v>
       </c>
-      <c r="B10" s="20"/>
-      <c r="C10" s="3" t="s">
+      <c r="B12" s="31"/>
+      <c r="C12" s="25" t="s">
         <v>727</v>
       </c>
-      <c r="D10" s="3"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="16" t="s">
+      <c r="D12" s="25"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="23" t="s">
         <v>703</v>
       </c>
-      <c r="B11" s="20"/>
-      <c r="C11" s="3" t="s">
+      <c r="B13" s="31"/>
+      <c r="C13" s="25" t="s">
         <v>728</v>
       </c>
-      <c r="D11" s="3"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="16" t="s">
+      <c r="D13" s="25"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="23" t="s">
         <v>704</v>
       </c>
-      <c r="B12" s="20"/>
-      <c r="C12" s="3" t="s">
+      <c r="B14" s="31"/>
+      <c r="C14" s="24" t="s">
         <v>729</v>
       </c>
-      <c r="D12" s="3"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="16" t="s">
+      <c r="D14" s="25"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="23" t="s">
         <v>705</v>
       </c>
-      <c r="B13" s="20"/>
-      <c r="C13" s="3" t="s">
+      <c r="B15" s="31"/>
+      <c r="C15" s="25" t="s">
         <v>730</v>
       </c>
-      <c r="D13" s="3"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="16" t="s">
+      <c r="D15" s="25"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="23" t="s">
         <v>706</v>
       </c>
-      <c r="B14" s="20"/>
-      <c r="C14" s="1" t="s">
+      <c r="B16" s="31" t="s">
         <v>731</v>
       </c>
-      <c r="D14" s="3"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="16" t="s">
+      <c r="C16" s="25" t="s">
+        <v>732</v>
+      </c>
+      <c r="D16" s="25"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="23" t="s">
         <v>707</v>
       </c>
-      <c r="B15" s="19"/>
-      <c r="C15" s="3" t="s">
-        <v>732</v>
-      </c>
-      <c r="D15" s="3"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="16" t="s">
+      <c r="B17" s="31"/>
+      <c r="C17" s="25" t="s">
+        <v>731</v>
+      </c>
+      <c r="D17" s="25"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="23" t="s">
         <v>708</v>
       </c>
-      <c r="B16" s="18" t="s">
+      <c r="B18" s="31"/>
+      <c r="C18" s="25" t="s">
         <v>733</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="D18" s="25"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="23" t="s">
+        <v>709</v>
+      </c>
+      <c r="B19" s="31"/>
+      <c r="C19" s="25" t="s">
         <v>734</v>
       </c>
-      <c r="D16" s="3"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="16" t="s">
-        <v>709</v>
-      </c>
-      <c r="B17" s="20"/>
-      <c r="C17" s="3" t="s">
-        <v>733</v>
-      </c>
-      <c r="D17" s="3"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="16" t="s">
+      <c r="D19" s="25"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="23" t="s">
         <v>710</v>
       </c>
-      <c r="B18" s="20"/>
-      <c r="C18" s="3" t="s">
+      <c r="B20" s="31"/>
+      <c r="C20" s="25" t="s">
         <v>735</v>
       </c>
-      <c r="D18" s="3"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="16" t="s">
+      <c r="D20" s="25"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="23" t="s">
         <v>711</v>
       </c>
-      <c r="B19" s="20"/>
-      <c r="C19" s="3" t="s">
+      <c r="B21" s="31" t="s">
         <v>736</v>
       </c>
-      <c r="D19" s="3"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="16" t="s">
+      <c r="C21" s="25" t="s">
+        <v>810</v>
+      </c>
+      <c r="D21" s="25"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="23" t="s">
         <v>712</v>
       </c>
-      <c r="B20" s="19"/>
-      <c r="C20" s="3" t="s">
+      <c r="B22" s="31"/>
+      <c r="C22" s="25" t="s">
+        <v>811</v>
+      </c>
+      <c r="D22" s="25"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="23" t="s">
+        <v>713</v>
+      </c>
+      <c r="B23" s="31" t="s">
         <v>737</v>
       </c>
-      <c r="D20" s="3"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="16" t="s">
-        <v>713</v>
-      </c>
-      <c r="B21" s="18" t="s">
+      <c r="C23" s="25" t="s">
         <v>738</v>
       </c>
-      <c r="C21" s="3" t="s">
-        <v>742</v>
-      </c>
-      <c r="D21" s="3"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="16" t="s">
+      <c r="D23" s="25"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="23" t="s">
         <v>714</v>
       </c>
-      <c r="B22" s="19"/>
-      <c r="C22" s="3" t="s">
-        <v>743</v>
-      </c>
-      <c r="D22" s="3"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="16" t="s">
-        <v>715</v>
-      </c>
-      <c r="B23" s="18" t="s">
+      <c r="B24" s="31"/>
+      <c r="C24" s="25" t="s">
         <v>739</v>
       </c>
-      <c r="C23" s="3" t="s">
-        <v>740</v>
-      </c>
-      <c r="D23" s="3"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="16" t="s">
-        <v>716</v>
-      </c>
-      <c r="B24" s="19"/>
-      <c r="C24" s="3" t="s">
-        <v>741</v>
-      </c>
-      <c r="D24" s="3"/>
+      <c r="D24" s="25"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="23" t="s">
+        <v>812</v>
+      </c>
+      <c r="B25" s="30" t="s">
+        <v>813</v>
+      </c>
+      <c r="C25" s="25" t="s">
+        <v>814</v>
+      </c>
+      <c r="D25" s="25"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="23" t="s">
+        <v>815</v>
+      </c>
+      <c r="B26" s="30"/>
+      <c r="C26" s="25" t="s">
+        <v>816</v>
+      </c>
+      <c r="D26" s="25"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="23" t="s">
+        <v>817</v>
+      </c>
+      <c r="B27" s="30"/>
+      <c r="C27" s="25" t="s">
+        <v>818</v>
+      </c>
+      <c r="D27" s="25"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="23" t="s">
+        <v>819</v>
+      </c>
+      <c r="B28" s="30" t="s">
+        <v>820</v>
+      </c>
+      <c r="C28" s="25" t="s">
+        <v>821</v>
+      </c>
+      <c r="D28" s="25"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="23" t="s">
+        <v>822</v>
+      </c>
+      <c r="B29" s="30"/>
+      <c r="C29" s="25" t="s">
+        <v>823</v>
+      </c>
+      <c r="D29" s="25"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" s="23" t="s">
+        <v>824</v>
+      </c>
+      <c r="B30" s="30" t="s">
+        <v>825</v>
+      </c>
+      <c r="C30" s="25" t="s">
+        <v>826</v>
+      </c>
+      <c r="D30" s="25"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" s="23" t="s">
+        <v>827</v>
+      </c>
+      <c r="B31" s="30"/>
+      <c r="C31" s="25" t="s">
+        <v>828</v>
+      </c>
+      <c r="D31" s="25"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" s="23" t="s">
+        <v>829</v>
+      </c>
+      <c r="B32" s="30"/>
+      <c r="C32" s="25" t="s">
+        <v>830</v>
+      </c>
+      <c r="D32" s="25"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" s="23" t="s">
+        <v>831</v>
+      </c>
+      <c r="B33" s="30"/>
+      <c r="C33" s="25" t="s">
+        <v>832</v>
+      </c>
+      <c r="D33" s="25"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" s="23" t="s">
+        <v>833</v>
+      </c>
+      <c r="B34" s="30" t="s">
+        <v>834</v>
+      </c>
+      <c r="C34" s="25" t="s">
+        <v>835</v>
+      </c>
+      <c r="D34" s="25"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" s="23" t="s">
+        <v>836</v>
+      </c>
+      <c r="B35" s="30"/>
+      <c r="C35" s="25" t="s">
+        <v>837</v>
+      </c>
+      <c r="D35" s="25"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" s="23" t="s">
+        <v>838</v>
+      </c>
+      <c r="B36" s="30"/>
+      <c r="C36" s="25" t="s">
+        <v>839</v>
+      </c>
+      <c r="D36" s="25"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" s="23" t="s">
+        <v>840</v>
+      </c>
+      <c r="B37" s="30"/>
+      <c r="C37" s="25" t="s">
+        <v>841</v>
+      </c>
+      <c r="D37" s="25"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" s="23" t="s">
+        <v>842</v>
+      </c>
+      <c r="B38" s="30" t="s">
+        <v>843</v>
+      </c>
+      <c r="C38" s="25" t="s">
+        <v>844</v>
+      </c>
+      <c r="D38" s="25"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" s="23" t="s">
+        <v>845</v>
+      </c>
+      <c r="B39" s="30"/>
+      <c r="C39" s="25" t="s">
+        <v>846</v>
+      </c>
+      <c r="D39" s="25"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" s="23" t="s">
+        <v>847</v>
+      </c>
+      <c r="B40" s="30"/>
+      <c r="C40" s="25" t="s">
+        <v>848</v>
+      </c>
+      <c r="D40" s="25"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" s="23" t="s">
+        <v>849</v>
+      </c>
+      <c r="B41" s="30"/>
+      <c r="C41" s="25" t="s">
+        <v>850</v>
+      </c>
+      <c r="D41" s="25"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" s="23" t="s">
+        <v>851</v>
+      </c>
+      <c r="B42" s="30"/>
+      <c r="C42" s="25" t="s">
+        <v>852</v>
+      </c>
+      <c r="D42" s="25"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" s="23" t="s">
+        <v>853</v>
+      </c>
+      <c r="B43" s="30"/>
+      <c r="C43" s="25" t="s">
+        <v>854</v>
+      </c>
+      <c r="D43" s="25"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" s="23" t="s">
+        <v>855</v>
+      </c>
+      <c r="B44" s="30"/>
+      <c r="C44" s="25" t="s">
+        <v>856</v>
+      </c>
+      <c r="D44" s="25"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45" s="23" t="s">
+        <v>857</v>
+      </c>
+      <c r="B45" s="30"/>
+      <c r="C45" s="25" t="s">
+        <v>858</v>
+      </c>
+      <c r="D45" s="25"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" s="23" t="s">
+        <v>859</v>
+      </c>
+      <c r="B46" s="30"/>
+      <c r="C46" s="25" t="s">
+        <v>948</v>
+      </c>
+      <c r="D46" s="25"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47" s="23" t="s">
+        <v>860</v>
+      </c>
+      <c r="B47" s="30"/>
+      <c r="C47" s="25" t="s">
+        <v>861</v>
+      </c>
+      <c r="D47" s="25"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48" s="23" t="s">
+        <v>862</v>
+      </c>
+      <c r="B48" s="30"/>
+      <c r="C48" s="25" t="s">
+        <v>863</v>
+      </c>
+      <c r="D48" s="25"/>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49" s="23" t="s">
+        <v>864</v>
+      </c>
+      <c r="B49" s="30"/>
+      <c r="C49" s="25" t="s">
+        <v>865</v>
+      </c>
+      <c r="D49" s="25"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50" s="23" t="s">
+        <v>866</v>
+      </c>
+      <c r="B50" s="30"/>
+      <c r="C50" s="25" t="s">
+        <v>867</v>
+      </c>
+      <c r="D50" s="25"/>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A51" s="27" t="s">
+        <v>868</v>
+      </c>
+      <c r="B51" s="30"/>
+      <c r="C51" s="25" t="s">
+        <v>869</v>
+      </c>
+      <c r="D51" s="25"/>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A52" s="23" t="s">
+        <v>952</v>
+      </c>
+      <c r="B52" s="30"/>
+      <c r="C52" s="38" t="s">
+        <v>953</v>
+      </c>
+      <c r="D52" s="25"/>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A53" s="23" t="s">
+        <v>870</v>
+      </c>
+      <c r="B53" s="30" t="s">
+        <v>871</v>
+      </c>
+      <c r="C53" s="25" t="s">
+        <v>872</v>
+      </c>
+      <c r="D53" s="25"/>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A54" s="23" t="s">
+        <v>873</v>
+      </c>
+      <c r="B54" s="30"/>
+      <c r="C54" s="25" t="s">
+        <v>874</v>
+      </c>
+      <c r="D54" s="25"/>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A55" s="23" t="s">
+        <v>875</v>
+      </c>
+      <c r="B55" s="30"/>
+      <c r="C55" s="25" t="s">
+        <v>876</v>
+      </c>
+      <c r="D55" s="25"/>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A56" s="23" t="s">
+        <v>877</v>
+      </c>
+      <c r="B56" s="30" t="s">
+        <v>878</v>
+      </c>
+      <c r="C56" s="25" t="s">
+        <v>879</v>
+      </c>
+      <c r="D56" s="25"/>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A57" s="23" t="s">
+        <v>880</v>
+      </c>
+      <c r="B57" s="30"/>
+      <c r="C57" s="25" t="s">
+        <v>881</v>
+      </c>
+      <c r="D57" s="25"/>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A58" s="23" t="s">
+        <v>882</v>
+      </c>
+      <c r="B58" s="30"/>
+      <c r="C58" s="25" t="s">
+        <v>883</v>
+      </c>
+      <c r="D58" s="25"/>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A59" s="23" t="s">
+        <v>884</v>
+      </c>
+      <c r="B59" s="30"/>
+      <c r="C59" s="25" t="s">
+        <v>885</v>
+      </c>
+      <c r="D59" s="25"/>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A60" s="23" t="s">
+        <v>886</v>
+      </c>
+      <c r="B60" s="30" t="s">
+        <v>887</v>
+      </c>
+      <c r="C60" s="25" t="s">
+        <v>888</v>
+      </c>
+      <c r="D60" s="25"/>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A61" s="23" t="s">
+        <v>889</v>
+      </c>
+      <c r="B61" s="30"/>
+      <c r="C61" s="25" t="s">
+        <v>890</v>
+      </c>
+      <c r="D61" s="25"/>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A62" s="23" t="s">
+        <v>891</v>
+      </c>
+      <c r="B62" s="30"/>
+      <c r="C62" s="25" t="s">
+        <v>892</v>
+      </c>
+      <c r="D62" s="25"/>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A63" s="23" t="s">
+        <v>893</v>
+      </c>
+      <c r="B63" s="30"/>
+      <c r="C63" s="25" t="s">
+        <v>894</v>
+      </c>
+      <c r="D63" s="25"/>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A64" s="23" t="s">
+        <v>895</v>
+      </c>
+      <c r="B64" s="30"/>
+      <c r="C64" s="25" t="s">
+        <v>896</v>
+      </c>
+      <c r="D64" s="25"/>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A65" s="23" t="s">
+        <v>897</v>
+      </c>
+      <c r="B65" s="30"/>
+      <c r="C65" s="25" t="s">
+        <v>898</v>
+      </c>
+      <c r="D65" s="25"/>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A66" s="23" t="s">
+        <v>899</v>
+      </c>
+      <c r="B66" s="30"/>
+      <c r="C66" s="25" t="s">
+        <v>900</v>
+      </c>
+      <c r="D66" s="25"/>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A67" s="23" t="s">
+        <v>901</v>
+      </c>
+      <c r="B67" s="30"/>
+      <c r="C67" s="25" t="s">
+        <v>902</v>
+      </c>
+      <c r="D67" s="25"/>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A68" s="23" t="s">
+        <v>903</v>
+      </c>
+      <c r="B68" s="30"/>
+      <c r="C68" s="25" t="s">
+        <v>904</v>
+      </c>
+      <c r="D68" s="25"/>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A69" s="23" t="s">
+        <v>905</v>
+      </c>
+      <c r="B69" s="30"/>
+      <c r="C69" s="25" t="s">
+        <v>906</v>
+      </c>
+      <c r="D69" s="25"/>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A70" s="23" t="s">
+        <v>907</v>
+      </c>
+      <c r="B70" s="30"/>
+      <c r="C70" s="25" t="s">
+        <v>908</v>
+      </c>
+      <c r="D70" s="25"/>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A71" s="23" t="s">
+        <v>909</v>
+      </c>
+      <c r="B71" s="30"/>
+      <c r="C71" s="25" t="s">
+        <v>910</v>
+      </c>
+      <c r="D71" s="25"/>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A72" s="23" t="s">
+        <v>911</v>
+      </c>
+      <c r="B72" s="30" t="s">
+        <v>912</v>
+      </c>
+      <c r="C72" s="25" t="s">
+        <v>913</v>
+      </c>
+      <c r="D72" s="25"/>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A73" s="23" t="s">
+        <v>914</v>
+      </c>
+      <c r="B73" s="30"/>
+      <c r="C73" s="25" t="s">
+        <v>915</v>
+      </c>
+      <c r="D73" s="25"/>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A74" s="23" t="s">
+        <v>916</v>
+      </c>
+      <c r="B74" s="30" t="s">
+        <v>917</v>
+      </c>
+      <c r="C74" s="25" t="s">
+        <v>918</v>
+      </c>
+      <c r="D74" s="25"/>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A75" s="23" t="s">
+        <v>919</v>
+      </c>
+      <c r="B75" s="30"/>
+      <c r="C75" s="25" t="s">
+        <v>949</v>
+      </c>
+      <c r="D75" s="25"/>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A76" s="23" t="s">
+        <v>920</v>
+      </c>
+      <c r="B76" s="26" t="s">
+        <v>921</v>
+      </c>
+      <c r="C76" s="25" t="s">
+        <v>950</v>
+      </c>
+      <c r="D76" s="25"/>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A77" s="23" t="s">
+        <v>922</v>
+      </c>
+      <c r="B77" s="30" t="s">
+        <v>923</v>
+      </c>
+      <c r="C77" s="25" t="s">
+        <v>924</v>
+      </c>
+      <c r="D77" s="25"/>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A78" s="23" t="s">
+        <v>925</v>
+      </c>
+      <c r="B78" s="30"/>
+      <c r="C78" s="25" t="s">
+        <v>926</v>
+      </c>
+      <c r="D78" s="25"/>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A79" s="23" t="s">
+        <v>927</v>
+      </c>
+      <c r="B79" s="30"/>
+      <c r="C79" s="25" t="s">
+        <v>928</v>
+      </c>
+      <c r="D79" s="25"/>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A80" s="23" t="s">
+        <v>929</v>
+      </c>
+      <c r="B80" s="30" t="s">
+        <v>930</v>
+      </c>
+      <c r="C80" s="25" t="s">
+        <v>931</v>
+      </c>
+      <c r="D80" s="25"/>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A81" s="23" t="s">
+        <v>932</v>
+      </c>
+      <c r="B81" s="30"/>
+      <c r="C81" s="25" t="s">
+        <v>933</v>
+      </c>
+      <c r="D81" s="25"/>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A82" s="23" t="s">
+        <v>934</v>
+      </c>
+      <c r="B82" s="30"/>
+      <c r="C82" s="25" t="s">
+        <v>935</v>
+      </c>
+      <c r="D82" s="25"/>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A83" s="23" t="s">
+        <v>936</v>
+      </c>
+      <c r="B83" s="30" t="s">
+        <v>937</v>
+      </c>
+      <c r="C83" s="25" t="s">
+        <v>938</v>
+      </c>
+      <c r="D83" s="25"/>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A84" s="23" t="s">
+        <v>939</v>
+      </c>
+      <c r="B84" s="30"/>
+      <c r="C84" s="25" t="s">
+        <v>940</v>
+      </c>
+      <c r="D84" s="25"/>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A85" s="23" t="s">
+        <v>941</v>
+      </c>
+      <c r="B85" s="30"/>
+      <c r="C85" s="25" t="s">
+        <v>942</v>
+      </c>
+      <c r="D85" s="25"/>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A86" s="23" t="s">
+        <v>951</v>
+      </c>
+      <c r="B86" s="30"/>
+      <c r="C86" s="28" t="s">
+        <v>954</v>
+      </c>
+      <c r="D86" s="25"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="18">
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="B4:B15"/>
     <mergeCell ref="B16:B20"/>
     <mergeCell ref="B21:B22"/>
     <mergeCell ref="B23:B24"/>
+    <mergeCell ref="B25:B27"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="B30:B33"/>
+    <mergeCell ref="B34:B37"/>
+    <mergeCell ref="B38:B52"/>
+    <mergeCell ref="B53:B55"/>
+    <mergeCell ref="B56:B59"/>
+    <mergeCell ref="B60:B71"/>
+    <mergeCell ref="B72:B73"/>
+    <mergeCell ref="B74:B75"/>
+    <mergeCell ref="B77:B79"/>
+    <mergeCell ref="B80:B82"/>
+    <mergeCell ref="B83:B86"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10178,7 +11707,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C10"/>
   <sheetViews>
@@ -10195,94 +11724,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="27" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
-        <v>745</v>
-      </c>
-      <c r="B1" s="15" t="s">
+      <c r="A1" s="14" t="s">
+        <v>741</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>760</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="15" t="s">
+        <v>761</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>762</v>
+      </c>
+      <c r="C2" s="3"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="15" t="s">
+        <v>752</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>763</v>
+      </c>
+      <c r="C3" s="3"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="15" t="s">
+        <v>753</v>
+      </c>
+      <c r="B4" s="13" t="s">
         <v>764</v>
       </c>
-      <c r="C1" s="15" t="s">
-        <v>744</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="16" t="s">
+      <c r="C4" s="3"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="15" t="s">
+        <v>754</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>768</v>
+      </c>
+      <c r="C5" s="3"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="15" t="s">
+        <v>755</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>769</v>
+      </c>
+      <c r="C6" s="3"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="15" t="s">
+        <v>756</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>770</v>
+      </c>
+      <c r="C7" s="3"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="15" t="s">
+        <v>757</v>
+      </c>
+      <c r="B8" s="13" t="s">
         <v>765</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="C8" s="3"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="15" t="s">
+        <v>758</v>
+      </c>
+      <c r="B9" s="13" t="s">
         <v>766</v>
       </c>
-      <c r="C2" s="3"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="16" t="s">
-        <v>756</v>
-      </c>
-      <c r="B3" s="14" t="s">
+      <c r="C9" s="3"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="15" t="s">
+        <v>759</v>
+      </c>
+      <c r="B10" s="13" t="s">
         <v>767</v>
-      </c>
-      <c r="C3" s="3"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="16" t="s">
-        <v>757</v>
-      </c>
-      <c r="B4" s="14" t="s">
-        <v>768</v>
-      </c>
-      <c r="C4" s="3"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="16" t="s">
-        <v>758</v>
-      </c>
-      <c r="B5" s="14" t="s">
-        <v>772</v>
-      </c>
-      <c r="C5" s="3"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="16" t="s">
-        <v>759</v>
-      </c>
-      <c r="B6" s="14" t="s">
-        <v>773</v>
-      </c>
-      <c r="C6" s="3"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="16" t="s">
-        <v>760</v>
-      </c>
-      <c r="B7" s="14" t="s">
-        <v>774</v>
-      </c>
-      <c r="C7" s="3"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="16" t="s">
-        <v>761</v>
-      </c>
-      <c r="B8" s="14" t="s">
-        <v>769</v>
-      </c>
-      <c r="C8" s="3"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="16" t="s">
-        <v>762</v>
-      </c>
-      <c r="B9" s="14" t="s">
-        <v>770</v>
-      </c>
-      <c r="C9" s="3"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="16" t="s">
-        <v>763</v>
-      </c>
-      <c r="B10" s="14" t="s">
-        <v>771</v>
       </c>
       <c r="C10" s="3"/>
     </row>
@@ -10293,7 +11822,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C16"/>
   <sheetViews>
@@ -10310,148 +11839,148 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="27" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="14" t="s">
+        <v>741</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>760</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="15" t="s">
+        <v>771</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>762</v>
+      </c>
+      <c r="C2" s="3"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="15" t="s">
+        <v>743</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>763</v>
+      </c>
+      <c r="C3" s="3"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="15" t="s">
+        <v>744</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>764</v>
+      </c>
+      <c r="C4" s="3"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="15" t="s">
         <v>745</v>
       </c>
-      <c r="B1" s="15" t="s">
-        <v>764</v>
-      </c>
-      <c r="C1" s="15" t="s">
-        <v>744</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="16" t="s">
-        <v>775</v>
-      </c>
-      <c r="B2" s="14" t="s">
-        <v>766</v>
-      </c>
-      <c r="C2" s="3"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="16" t="s">
+      <c r="B5" s="13" t="s">
+        <v>768</v>
+      </c>
+      <c r="C5" s="3"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="15" t="s">
+        <v>746</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>769</v>
+      </c>
+      <c r="C6" s="3"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="15" t="s">
         <v>747</v>
       </c>
-      <c r="B3" s="14" t="s">
-        <v>767</v>
-      </c>
-      <c r="C3" s="3"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="16" t="s">
+      <c r="B7" s="13" t="s">
+        <v>770</v>
+      </c>
+      <c r="C7" s="3"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="15" t="s">
         <v>748</v>
       </c>
-      <c r="B4" s="14" t="s">
-        <v>768</v>
-      </c>
-      <c r="C4" s="3"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="16" t="s">
+      <c r="B8" s="13" t="s">
+        <v>788</v>
+      </c>
+      <c r="C8" s="3"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="15" t="s">
         <v>749</v>
       </c>
-      <c r="B5" s="14" t="s">
-        <v>772</v>
-      </c>
-      <c r="C5" s="3"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="16" t="s">
+      <c r="B9" s="13" t="s">
+        <v>789</v>
+      </c>
+      <c r="C9" s="3"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="15" t="s">
         <v>750</v>
       </c>
-      <c r="B6" s="14" t="s">
-        <v>773</v>
-      </c>
-      <c r="C6" s="3"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="16" t="s">
-        <v>751</v>
-      </c>
-      <c r="B7" s="14" t="s">
-        <v>774</v>
-      </c>
-      <c r="C7" s="3"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="16" t="s">
-        <v>752</v>
-      </c>
-      <c r="B8" s="14" t="s">
+      <c r="B10" s="13" t="s">
+        <v>790</v>
+      </c>
+      <c r="C10" s="3"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="15" t="s">
+        <v>782</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>791</v>
+      </c>
+      <c r="C11" s="3"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="15" t="s">
+        <v>783</v>
+      </c>
+      <c r="B12" s="16" t="s">
         <v>792</v>
       </c>
-      <c r="C8" s="3"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="16" t="s">
-        <v>753</v>
-      </c>
-      <c r="B9" s="14" t="s">
+      <c r="C12" s="3"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="15" t="s">
+        <v>784</v>
+      </c>
+      <c r="B13" s="16" t="s">
         <v>793</v>
       </c>
-      <c r="C9" s="3"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="16" t="s">
-        <v>754</v>
-      </c>
-      <c r="B10" s="14" t="s">
+      <c r="C13" s="3"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="15" t="s">
+        <v>785</v>
+      </c>
+      <c r="B14" s="16" t="s">
         <v>794</v>
       </c>
-      <c r="C10" s="3"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="16" t="s">
+      <c r="C14" s="3"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="15" t="s">
         <v>786</v>
       </c>
-      <c r="B11" s="17" t="s">
+      <c r="B15" s="16" t="s">
         <v>795</v>
       </c>
-      <c r="C11" s="3"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="16" t="s">
+      <c r="C15" s="3"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="15" t="s">
         <v>787</v>
       </c>
-      <c r="B12" s="17" t="s">
+      <c r="B16" s="16" t="s">
         <v>796</v>
-      </c>
-      <c r="C12" s="3"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="16" t="s">
-        <v>788</v>
-      </c>
-      <c r="B13" s="17" t="s">
-        <v>797</v>
-      </c>
-      <c r="C13" s="3"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="16" t="s">
-        <v>789</v>
-      </c>
-      <c r="B14" s="17" t="s">
-        <v>798</v>
-      </c>
-      <c r="C14" s="3"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="16" t="s">
-        <v>790</v>
-      </c>
-      <c r="B15" s="17" t="s">
-        <v>799</v>
-      </c>
-      <c r="C15" s="3"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="16" t="s">
-        <v>791</v>
-      </c>
-      <c r="B16" s="17" t="s">
-        <v>800</v>
       </c>
       <c r="C16" s="3"/>
     </row>
@@ -10462,7 +11991,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D6"/>
   <sheetViews>
@@ -10480,31 +12009,31 @@
       <c r="A1" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="32" t="s">
         <v>199</v>
       </c>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>194</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="32" t="s">
         <v>197</v>
       </c>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>190</v>
       </c>
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="32" t="s">
         <v>191</v>
       </c>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
@@ -10521,20 +12050,20 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="22" t="s">
+      <c r="A5" s="33" t="s">
         <v>195</v>
       </c>
-      <c r="B5" s="22"/>
-      <c r="C5" s="22"/>
-      <c r="D5" s="22"/>
+      <c r="B5" s="33"/>
+      <c r="C5" s="33"/>
+      <c r="D5" s="33"/>
     </row>
     <row r="6" spans="1:4" ht="66.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="23" t="s">
+      <c r="A6" s="34" t="s">
         <v>196</v>
       </c>
-      <c r="B6" s="23"/>
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
+      <c r="B6" s="34"/>
+      <c r="C6" s="34"/>
+      <c r="D6" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -10550,7 +12079,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D17"/>
   <sheetViews>
@@ -10812,7 +12341,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D9"/>
   <sheetViews>
@@ -10960,210 +12489,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D13"/>
-  <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="8" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="39.625" style="2" customWidth="1"/>
-    <col min="5" max="16384" width="9" style="2"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="27" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="27" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="27" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="27" x14ac:dyDescent="0.3">
-      <c r="A13" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>